<commit_message>
Final proyect commit with analysis working
</commit_message>
<xml_diff>
--- a/final_df_bike_hires.xlsx
+++ b/final_df_bike_hires.xlsx
@@ -597,7 +597,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -4906,7 +4906,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I144" t="n">
@@ -5805,7 +5805,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I173" t="n">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I187" t="n">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I191" t="n">
@@ -6828,7 +6828,7 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I206" t="n">
@@ -6890,7 +6890,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I208" t="n">
@@ -7231,7 +7231,7 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I219" t="n">
@@ -8006,7 +8006,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I244" t="n">
@@ -8068,7 +8068,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I246" t="n">
@@ -10331,7 +10331,7 @@
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I319" t="n">
@@ -10579,7 +10579,7 @@
       </c>
       <c r="H327" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I327" t="n">
@@ -10765,7 +10765,7 @@
       </c>
       <c r="H333" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I333" t="n">
@@ -10796,7 +10796,7 @@
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I334" t="n">
@@ -10982,7 +10982,7 @@
       </c>
       <c r="H340" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I340" t="n">
@@ -11416,7 +11416,7 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I354" t="n">
@@ -12935,7 +12935,7 @@
       </c>
       <c r="H403" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I403" t="n">
@@ -13276,7 +13276,7 @@
       </c>
       <c r="H414" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I414" t="n">
@@ -13369,7 +13369,7 @@
       </c>
       <c r="H417" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I417" t="n">
@@ -13803,7 +13803,7 @@
       </c>
       <c r="H431" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I431" t="n">
@@ -14454,7 +14454,7 @@
       </c>
       <c r="H452" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I452" t="n">
@@ -15322,7 +15322,7 @@
       </c>
       <c r="H480" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I480" t="n">
@@ -15818,7 +15818,7 @@
       </c>
       <c r="H496" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I496" t="n">
@@ -16562,7 +16562,7 @@
       </c>
       <c r="H520" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I520" t="n">
@@ -17461,7 +17461,7 @@
       </c>
       <c r="H549" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I549" t="n">
@@ -17709,7 +17709,7 @@
       </c>
       <c r="H557" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I557" t="n">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="H579" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I579" t="n">
@@ -19228,7 +19228,7 @@
       </c>
       <c r="H606" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I606" t="n">
@@ -19786,7 +19786,7 @@
       </c>
       <c r="H624" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I624" t="n">
@@ -20313,7 +20313,7 @@
       </c>
       <c r="H641" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I641" t="n">
@@ -20530,7 +20530,7 @@
       </c>
       <c r="H648" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I648" t="n">
@@ -20747,7 +20747,7 @@
       </c>
       <c r="H655" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I655" t="n">
@@ -20964,7 +20964,7 @@
       </c>
       <c r="H662" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I662" t="n">
@@ -21398,7 +21398,7 @@
       </c>
       <c r="H676" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I676" t="n">
@@ -22049,7 +22049,7 @@
       </c>
       <c r="H697" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I697" t="n">
@@ -22266,7 +22266,7 @@
       </c>
       <c r="H704" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I704" t="n">
@@ -23568,7 +23568,7 @@
       </c>
       <c r="H746" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I746" t="n">
@@ -24002,7 +24002,7 @@
       </c>
       <c r="H760" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I760" t="n">
@@ -24219,7 +24219,7 @@
       </c>
       <c r="H767" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I767" t="n">
@@ -24436,7 +24436,7 @@
       </c>
       <c r="H774" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I774" t="n">
@@ -25211,7 +25211,7 @@
       </c>
       <c r="H799" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I799" t="n">
@@ -27350,7 +27350,7 @@
       </c>
       <c r="H868" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I868" t="n">
@@ -27598,7 +27598,7 @@
       </c>
       <c r="H876" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I876" t="n">
@@ -27970,7 +27970,7 @@
       </c>
       <c r="H888" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I888" t="n">
@@ -28528,7 +28528,7 @@
       </c>
       <c r="H906" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I906" t="n">
@@ -29210,7 +29210,7 @@
       </c>
       <c r="H928" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I928" t="n">
@@ -29396,7 +29396,7 @@
       </c>
       <c r="H934" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I934" t="n">
@@ -29427,7 +29427,7 @@
       </c>
       <c r="H935" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I935" t="n">
@@ -29892,7 +29892,7 @@
       </c>
       <c r="H950" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I950" t="n">
@@ -30977,7 +30977,7 @@
       </c>
       <c r="H985" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I985" t="n">
@@ -32465,7 +32465,7 @@
       </c>
       <c r="H1033" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1033" t="n">
@@ -34294,7 +34294,7 @@
       </c>
       <c r="H1092" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1092" t="n">
@@ -35069,7 +35069,7 @@
       </c>
       <c r="H1117" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1117" t="n">
@@ -36123,7 +36123,7 @@
       </c>
       <c r="H1151" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1151" t="n">
@@ -36309,7 +36309,7 @@
       </c>
       <c r="H1157" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1157" t="n">
@@ -36371,7 +36371,7 @@
       </c>
       <c r="H1159" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1159" t="n">
@@ -37177,7 +37177,7 @@
       </c>
       <c r="H1185" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1185" t="n">
@@ -37239,7 +37239,7 @@
       </c>
       <c r="H1187" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1187" t="n">
@@ -37270,7 +37270,7 @@
       </c>
       <c r="H1188" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1188" t="n">
@@ -38417,7 +38417,7 @@
       </c>
       <c r="H1225" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1225" t="n">
@@ -38510,7 +38510,7 @@
       </c>
       <c r="H1228" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1228" t="n">
@@ -38696,7 +38696,7 @@
       </c>
       <c r="H1234" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1234" t="n">
@@ -41796,7 +41796,7 @@
       </c>
       <c r="H1334" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1334" t="n">
@@ -42664,7 +42664,7 @@
       </c>
       <c r="H1362" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1362" t="n">
@@ -43315,7 +43315,7 @@
       </c>
       <c r="H1383" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1383" t="n">
@@ -45888,7 +45888,7 @@
       </c>
       <c r="H1466" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1466" t="n">
@@ -46322,7 +46322,7 @@
       </c>
       <c r="H1480" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1480" t="n">
@@ -46756,7 +46756,7 @@
       </c>
       <c r="H1494" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1494" t="n">
@@ -46973,7 +46973,7 @@
       </c>
       <c r="H1501" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1501" t="n">
@@ -47283,7 +47283,7 @@
       </c>
       <c r="H1511" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1511" t="n">
@@ -47500,7 +47500,7 @@
       </c>
       <c r="H1518" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1518" t="n">
@@ -47531,7 +47531,7 @@
       </c>
       <c r="H1519" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1519" t="n">
@@ -48926,7 +48926,7 @@
       </c>
       <c r="H1564" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1564" t="n">
@@ -50290,7 +50290,7 @@
       </c>
       <c r="H1608" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1608" t="n">
@@ -50631,7 +50631,7 @@
       </c>
       <c r="H1619" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1619" t="n">
@@ -50724,7 +50724,7 @@
       </c>
       <c r="H1622" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1622" t="n">
@@ -51778,7 +51778,7 @@
       </c>
       <c r="H1656" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1656" t="n">
@@ -52181,7 +52181,7 @@
       </c>
       <c r="H1669" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1669" t="n">
@@ -54010,7 +54010,7 @@
       </c>
       <c r="H1728" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1728" t="n">
@@ -54134,7 +54134,7 @@
       </c>
       <c r="H1732" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1732" t="n">
@@ -54165,7 +54165,7 @@
       </c>
       <c r="H1733" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1733" t="n">
@@ -54568,7 +54568,7 @@
       </c>
       <c r="H1746" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1746" t="n">
@@ -54599,7 +54599,7 @@
       </c>
       <c r="H1747" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1747" t="n">
@@ -54816,7 +54816,7 @@
       </c>
       <c r="H1754" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1754" t="n">
@@ -55002,7 +55002,7 @@
       </c>
       <c r="H1760" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1760" t="n">
@@ -55219,7 +55219,7 @@
       </c>
       <c r="H1767" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1767" t="n">
@@ -55653,7 +55653,7 @@
       </c>
       <c r="H1781" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1781" t="n">
@@ -55870,7 +55870,7 @@
       </c>
       <c r="H1788" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1788" t="n">
@@ -56521,7 +56521,7 @@
       </c>
       <c r="H1809" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1809" t="n">
@@ -56738,7 +56738,7 @@
       </c>
       <c r="H1816" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1816" t="n">
@@ -57017,7 +57017,7 @@
       </c>
       <c r="H1825" t="inlineStr">
         <is>
-          <t>The day is unusual</t>
+          <t>The day is significantly unusual</t>
         </is>
       </c>
       <c r="I1825" t="n">

</xml_diff>